<commit_message>
create minihabits and base on week
</commit_message>
<xml_diff>
--- a/september.xlsx
+++ b/september.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGits\minihabits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGits\MiniHabits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD2A501-E7DE-4E5E-933E-402E16E15654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8563337-3400-4AC9-922A-49E527CEE48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Read 2 pages English novel</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -44,6 +44,10 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>play basketball</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -384,7 +388,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -444,10 +448,28 @@
       <c r="A6" s="1">
         <v>45556</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45557</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>